<commit_message>
Added writing ramp rates to p_gnn (p.u./min) when the parameter is given in lines table.
</commit_message>
<xml_diff>
--- a/input/additional-lines1.xlsx
+++ b/input/additional-lines1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="18">
   <si>
     <t xml:space="preserve">Node/Line</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve">National Trends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI00-SE03</t>
   </si>
 </sst>
 </file>
@@ -201,8 +204,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF232627"/>
-          <bgColor rgb="FFFCFCFC"/>
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -222,7 +225,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +387,7 @@
       <c r="F6" s="1" t="n">
         <v>2040</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>1984</v>
       </c>
       <c r="H6" s="1" t="n">
@@ -410,7 +413,7 @@
       <c r="F7" s="1" t="n">
         <v>2040</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>1984</v>
       </c>
       <c r="H7" s="3" t="n">
@@ -678,22 +681,56 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G18" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H18" s="3" t="n">
+        <v>500</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <v>-1200</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3"/>
@@ -913,11 +950,9 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="1"/>
-      <c r="G44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="1"/>
-      <c r="G45" s="0"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H17"/>

</xml_diff>

<commit_message>
Added H2 in SE01.
</commit_message>
<xml_diff>
--- a/input/additional-lines1.xlsx
+++ b/input/additional-lines1.xlsx
@@ -225,7 +225,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -703,7 +703,7 @@
         <v>1984</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>500</v>
+        <v>700</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
updated electrolysis, EV FI00. Added Estlink 3.
</commit_message>
<xml_diff>
--- a/input/additional-lines1.xlsx
+++ b/input/additional-lines1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
   <si>
     <t xml:space="preserve">Node/Line</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t xml:space="preserve">FI00-SE03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EE00-FI00</t>
   </si>
 </sst>
 </file>
@@ -225,7 +228,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,7 +394,7 @@
         <v>1984</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>3000</v>
+        <v>2900</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,7 +420,7 @@
         <v>1984</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>-3000</v>
+        <v>-2900</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,22 +736,56 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G20" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>1700</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G21" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H21" s="3" t="n">
+        <v>-1700</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3"/>

</xml_diff>

<commit_message>
Added EV to FR00. Added reinforcement line NOM1-NON1 (See Nordic grid development perspective 2023).
</commit_message>
<xml_diff>
--- a/input/additional-lines1.xlsx
+++ b/input/additional-lines1.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Line" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Line" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Line!$A$1:$H$17</definedName>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="20">
   <si>
     <t xml:space="preserve">Node/Line</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">EE00-FI00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOM1-NON1</t>
   </si>
 </sst>
 </file>
@@ -200,7 +203,7 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -208,7 +211,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -220,6 +223,112 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -228,7 +337,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -788,22 +897,56 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>2100</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G23" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>-2100</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>

</xml_diff>

<commit_message>
Updated capacities 2030, interconnections SE04 2030.
</commit_message>
<xml_diff>
--- a/input/additional-lines1.xlsx
+++ b/input/additional-lines1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="24">
   <si>
     <t xml:space="preserve">Node/Line</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
     <t xml:space="preserve">DE00-PL00</t>
   </si>
   <si>
@@ -84,6 +87,15 @@
   </si>
   <si>
     <t xml:space="preserve">NOM1-NON1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE00-SE04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYNDP economic needs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL00-SE04</t>
   </si>
 </sst>
 </file>
@@ -334,10 +346,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,6 +360,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="24.74"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -375,22 +388,25 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>2030</v>
@@ -404,19 +420,19 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>2030</v>
@@ -430,19 +446,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>2040</v>
@@ -456,19 +472,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>2040</v>
@@ -482,19 +498,19 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>2040</v>
@@ -508,19 +524,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>2040</v>
@@ -534,19 +550,19 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>2030</v>
@@ -560,19 +576,19 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>2030</v>
@@ -586,19 +602,19 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F10" s="3" t="n">
         <v>2040</v>
@@ -612,19 +628,19 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F11" s="3" t="n">
         <v>2040</v>
@@ -638,19 +654,19 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F12" s="3" t="n">
         <v>2025</v>
@@ -664,19 +680,19 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F13" s="3" t="n">
         <v>2025</v>
@@ -690,19 +706,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F14" s="3" t="n">
         <v>2030</v>
@@ -716,19 +732,19 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" s="3" t="n">
         <v>2030</v>
@@ -742,19 +758,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F16" s="3" t="n">
         <v>2040</v>
@@ -768,19 +784,19 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F17" s="3" t="n">
         <v>2040</v>
@@ -794,19 +810,19 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E18" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F18" s="3" t="n">
         <v>2025</v>
@@ -820,19 +836,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F19" s="3" t="n">
         <v>2025</v>
@@ -846,19 +862,19 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F20" s="3" t="n">
         <v>2040</v>
@@ -872,19 +888,19 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F21" s="3" t="n">
         <v>2040</v>
@@ -898,19 +914,19 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F22" s="3" t="n">
         <v>2040</v>
@@ -924,19 +940,19 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F23" s="3" t="n">
         <v>2040</v>
@@ -949,76 +965,236 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G24" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H24" s="3" t="n">
+        <v>1315</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G25" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>-1315</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G26" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H26" s="3" t="n">
+        <v>1315</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="A27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G27" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H27" s="3" t="n">
+        <v>-1315</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="A28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>1300</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
+      <c r="A29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="3" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G29" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H29" s="3" t="n">
+        <v>-1300</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
+      <c r="A30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G30" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H30" s="3" t="n">
+        <v>1300</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>-1300</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>

</xml_diff>

<commit_message>
Updated transmission capacity e.g. FR00-ES00.
</commit_message>
<xml_diff>
--- a/input/additional-lines1.xlsx
+++ b/input/additional-lines1.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Line!$A$1:$H$17</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Line!$A$1:$I$43</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="37">
   <si>
     <t xml:space="preserve">Node/Line</t>
   </si>
@@ -62,40 +62,79 @@
     <t xml:space="preserve">Interconnection</t>
   </si>
   <si>
+    <t xml:space="preserve">National Trends</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference Grid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Import Capacity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FI00-SE03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOS0-UK00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No North Sea link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES00-FR00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Biscay gulf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE00-FR00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE00-UK00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NeuConnect cable</t>
+  </si>
+  <si>
     <t xml:space="preserve">Distributed Energy</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference Grid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Import Capacity</t>
+    <t xml:space="preserve">Global Ambition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE00-SE04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYNDP economic needs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL00-SE04</t>
   </si>
   <si>
     <t xml:space="preserve">FI00-SE01</t>
   </si>
   <si>
-    <t xml:space="preserve">Global Ambition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National Trends</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FI00-SE03</t>
-  </si>
-  <si>
     <t xml:space="preserve">EE00-FI00</t>
   </si>
   <si>
+    <t xml:space="preserve">Estlink 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">NOM1-NON1</t>
   </si>
   <si>
-    <t xml:space="preserve">DE00-SE04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYNDP economic needs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PL00-SE04</t>
+    <t xml:space="preserve">Navarra-Landes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DE00-FR00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vigy-Uchtelfangen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE00-NL00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upgrade Vaneyck-Maasbracht</t>
   </si>
 </sst>
 </file>
@@ -136,12 +175,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF6600"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD4EA6B"/>
+        <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -185,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,6 +253,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -211,7 +270,23 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD4EA6B"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF8000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -228,6 +303,66 @@
       </fill>
     </dxf>
   </dxfs>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFD4EA6B"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF8000"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -346,10 +481,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -409,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="G2" s="3" t="n">
         <v>1984</v>
@@ -435,7 +570,7 @@
         <v>13</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="G3" s="3" t="n">
         <v>1984</v>
@@ -445,8 +580,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>10</v>
@@ -461,18 +596,18 @@
         <v>13</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="G4" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>2000</v>
+        <v>700</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
+      <c r="A5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>14</v>
@@ -487,183 +622,195 @@
         <v>13</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="G5" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>-3000</v>
+        <v>-1200</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="1" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G6" s="1" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H6" s="1" t="n">
-        <v>2900</v>
+      <c r="F6" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H6" s="3" t="n">
+        <v>1400</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="1" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G7" s="1" t="n">
+      <c r="F7" s="3" t="n">
+        <v>2025</v>
+      </c>
+      <c r="G7" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>-2900</v>
+        <v>-1400</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="G8" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>2000</v>
+        <v>2800</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="G9" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>-3000</v>
+        <v>-2800</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="G10" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>2000</v>
+        <v>650</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="3" t="s">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>2040</v>
+        <v>2025</v>
       </c>
       <c r="G11" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>-3000</v>
+        <v>-1800</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -675,21 +822,24 @@
         <v>1984</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>2000</v>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>13</v>
@@ -701,7 +851,10 @@
         <v>1984</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>-3000</v>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -715,7 +868,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -741,7 +894,7 @@
         <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
@@ -767,13 +920,13 @@
         <v>11</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="G16" s="3" t="n">
         <v>1984</v>
@@ -793,13 +946,13 @@
         <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="3" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="G17" s="3" t="n">
         <v>1984</v>
@@ -809,8 +962,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>18</v>
+      <c r="A18" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>10</v>
@@ -819,24 +972,24 @@
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="3" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="G18" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H18" s="3" t="n">
-        <v>700</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
-        <v>18</v>
+      <c r="A19" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>14</v>
@@ -845,24 +998,24 @@
         <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="3" t="n">
-        <v>2025</v>
+        <v>2030</v>
       </c>
       <c r="G19" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>-1200</v>
+        <v>-3000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>19</v>
+      <c r="A20" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>10</v>
@@ -871,24 +1024,27 @@
         <v>11</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="3" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="G20" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H20" s="3" t="n">
-        <v>1700</v>
+        <v>1315</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>19</v>
+      <c r="A21" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>14</v>
@@ -897,76 +1053,85 @@
         <v>11</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F21" s="3" t="n">
-        <v>2040</v>
+        <v>2030</v>
       </c>
       <c r="G21" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H21" s="3" t="n">
-        <v>-1700</v>
+        <v>-1315</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G22" s="3" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H22" s="3" t="n">
-        <v>2100</v>
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>1300</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G23" s="3" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H23" s="3" t="n">
-        <v>-2100</v>
+      <c r="A23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>2030</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>-1300</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>21</v>
+      <c r="A24" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>10</v>
@@ -975,27 +1140,24 @@
         <v>11</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="G24" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H24" s="3" t="n">
-        <v>1315</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>22</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>21</v>
+      <c r="A25" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>14</v>
@@ -1004,85 +1166,76 @@
         <v>11</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="G25" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H25" s="3" t="n">
-        <v>-1315</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>22</v>
+        <v>-3000</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G26" s="3" t="n">
-        <v>1984</v>
-      </c>
-      <c r="H26" s="3" t="n">
-        <v>1315</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>22</v>
+      <c r="F26" s="1" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>2900</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F27" s="3" t="n">
-        <v>2040</v>
-      </c>
-      <c r="G27" s="3" t="n">
+      <c r="F27" s="1" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G27" s="1" t="n">
         <v>1984</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>-1315</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>22</v>
+        <v>-2900</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="s">
-        <v>23</v>
+      <c r="A28" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>10</v>
@@ -1091,27 +1244,24 @@
         <v>11</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="G28" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H28" s="3" t="n">
-        <v>1300</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>22</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>23</v>
+      <c r="A29" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>14</v>
@@ -1120,27 +1270,24 @@
         <v>11</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="3" t="n">
-        <v>2030</v>
+        <v>2040</v>
       </c>
       <c r="G29" s="3" t="n">
         <v>1984</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>-1300</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>22</v>
+        <v>-3000</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="s">
-        <v>23</v>
+      <c r="A30" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>10</v>
@@ -1161,15 +1308,12 @@
         <v>1984</v>
       </c>
       <c r="H30" s="3" t="n">
-        <v>1300</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>22</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="s">
-        <v>23</v>
+      <c r="A31" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>14</v>
@@ -1190,128 +1334,417 @@
         <v>1984</v>
       </c>
       <c r="H31" s="3" t="n">
+        <v>-3000</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G32" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H32" s="3" t="n">
+        <v>1700</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G33" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H33" s="3" t="n">
+        <v>-1700</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G34" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G35" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>-2100</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G36" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H36" s="3" t="n">
+        <v>1315</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G37" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>-1315</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G38" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H38" s="3" t="n">
+        <v>1300</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="3" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G39" s="3" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H39" s="3" t="n">
         <v>-1300</v>
       </c>
-      <c r="I31" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
+      <c r="I39" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+      <c r="A40" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G40" s="5" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H40" s="5" t="n">
+        <v>6500</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+      <c r="A41" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G41" s="5" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H41" s="5" t="n">
+        <v>-6500</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="A42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G42" s="5" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H42" s="5" t="n">
+        <v>4500</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="A43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G43" s="5" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H43" s="5" t="n">
+        <v>-4500</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F44" s="1"/>
+      <c r="A44" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G44" s="5" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H44" s="5" t="n">
+        <v>3400</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F45" s="1"/>
+      <c r="A45" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="5" t="n">
+        <v>2040</v>
+      </c>
+      <c r="G45" s="5" t="n">
+        <v>1984</v>
+      </c>
+      <c r="H45" s="5" t="n">
+        <v>-3400</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H17"/>
+  <autoFilter ref="A1:I43"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>